<commit_message>
-xlsx --> png executed via excel2png lib (updated requirement). -sample image file in data folder uploaded, -minor change in Global Variables section: unified quotation/single quatation notation
</commit_message>
<xml_diff>
--- a/data/Template.xlsx
+++ b/data/Template.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Main!$D$1:$P$17</definedName>
+    <definedName name="Output_Area">Main!$D$1:$R$18</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -30,49 +30,49 @@
     <t>Nasdaq OMX Baltic Price Performance Highlights</t>
   </si>
   <si>
-    <t>GRZ1R</t>
-  </si>
-  <si>
-    <t>KNR1L</t>
-  </si>
-  <si>
-    <t>SNG1L</t>
+    <t>RKB1R</t>
   </si>
   <si>
     <t>SKN1T</t>
   </si>
   <si>
+    <t>OLF1R</t>
+  </si>
+  <si>
+    <t>ARC1T</t>
+  </si>
+  <si>
+    <t>IVL1L</t>
+  </si>
+  <si>
+    <t>Worst Performers</t>
+  </si>
+  <si>
+    <t>TSM1T</t>
+  </si>
+  <si>
+    <t>SFG1T</t>
+  </si>
+  <si>
     <t>EWA1L</t>
   </si>
   <si>
-    <t>Worst Performers</t>
-  </si>
-  <si>
-    <t>BLT1T</t>
-  </si>
-  <si>
-    <t>SFG1T</t>
-  </si>
-  <si>
-    <t>AMG1L</t>
-  </si>
-  <si>
-    <t>HAE1T</t>
-  </si>
-  <si>
-    <t>EEG1T</t>
+    <t>NTU1L</t>
+  </si>
+  <si>
+    <t>SAF1R</t>
   </si>
   <si>
     <t>Start date</t>
   </si>
   <si>
-    <t>2019.05.21</t>
+    <t>2019.05.31</t>
   </si>
   <si>
     <t>End date</t>
   </si>
   <si>
-    <t>2019.05.14</t>
+    <t>2019.05.24</t>
   </si>
 </sst>
 </file>
@@ -328,19 +328,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>BLT1T</c:v>
+                  <c:v>TSM1T</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>SFG1T</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>AMG1L</c:v>
+                  <c:v>EWA1L</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>HAE1T</c:v>
+                  <c:v>NTU1L</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>EEG1T</c:v>
+                  <c:v>SAF1R</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -352,19 +352,19 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-0.24148606811145501</c:v>
+                  <c:v>-6.5116279069767496E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.111969111969112</c:v>
+                  <c:v>-4.8888888888888843E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.0000000000000037E-2</c:v>
+                  <c:v>-4.5161290322580601E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-4.8625792811839409E-2</c:v>
+                  <c:v>-3.7499999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.9548022598870088E-2</c:v>
+                  <c:v>-3.067484662576676E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -379,11 +379,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="114248416"/>
-        <c:axId val="114248976"/>
+        <c:axId val="107287968"/>
+        <c:axId val="107288528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="114248416"/>
+        <c:axId val="107287968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +426,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114248976"/>
+        <c:crossAx val="107288528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114248976"/>
+        <c:axId val="107288528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,7 +471,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="114248416"/>
+        <c:crossAx val="107287968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -642,19 +642,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>GRZ1R</c:v>
+                  <c:v>RKB1R</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>KNR1L</c:v>
+                  <c:v>SKN1T</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>SNG1L</c:v>
+                  <c:v>OLF1R</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>SKN1T</c:v>
+                  <c:v>ARC1T</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>EWA1L</c:v>
+                  <c:v>IVL1L</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -666,19 +666,19 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.98</c:v>
+                  <c:v>0.19696969696969691</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8901098901098869E-2</c:v>
+                  <c:v>0.15384615384615399</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9545454545454447E-2</c:v>
+                  <c:v>0.1316725978647687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.8341013824884731E-2</c:v>
+                  <c:v>5.454545454545439E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1428571428571425E-2</c:v>
+                  <c:v>3.603603603603607E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -693,11 +693,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="115902720"/>
-        <c:axId val="115903280"/>
+        <c:axId val="108628656"/>
+        <c:axId val="108629216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115902720"/>
+        <c:axId val="108628656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -740,7 +740,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115903280"/>
+        <c:crossAx val="108629216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -748,7 +748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115903280"/>
+        <c:axId val="108629216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -785,7 +785,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115902720"/>
+        <c:crossAx val="108628656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -806,13 +806,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -836,13 +836,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1130,108 +1130,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="2.7109375" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1.98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.19696969696969691</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>9.8901098901098869E-2</v>
-      </c>
-      <c r="J3" s="3" t="str">
+        <v>0.15384615384615399</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="K3" s="3" t="str">
         <f>B19&amp;" - "&amp;B18</f>
-        <v>2019.05.14 - 2019.05.21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2019.05.24 - 2019.05.31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>7.9545454545454447E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.1316725978647687</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>7.8341013824884731E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.454545454545439E-2</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>7.1428571428571425E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.603603603603607E-2</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.24148606811145501</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-6.5116279069767496E-2</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>-0.111969111969112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-4.8888888888888843E-2</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>-5.0000000000000037E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-4.5161290322580601E-2</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>-4.8625792811839409E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-3.7499999999999978E-2</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>-3.9548022598870088E-2</v>
-      </c>
+        <v>-3.067484662576676E-2</v>
+      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1251,7 +1265,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resolve #14 -Enabled program to work at any day; -Automatically finds working date pair separated by week; -unified quotation notation accross the program -minor docstring changes
</commit_message>
<xml_diff>
--- a/data/Template.xlsx
+++ b/data/Template.xlsx
@@ -223,7 +223,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="lt-LT"/>
               </a:p>
@@ -338,7 +338,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
@@ -386,7 +386,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
@@ -522,7 +522,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="lt-LT"/>
               </a:p>
@@ -637,7 +637,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
@@ -685,7 +685,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
@@ -1054,22 +1054,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SAF1R</t>
+          <t>RKB1R</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>0.2482758620689656</v>
+        <v>0.1969696969696969</v>
       </c>
       <c r="C2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>KA11R</t>
+          <t>SKN1T</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0.2307692307692308</v>
+        <v>0.153846153846154</v>
       </c>
       <c r="C3" s="1" t="n"/>
       <c r="K3" s="3">
@@ -1080,33 +1080,33 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RRR1R</t>
+          <t>OLF1R</t>
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.07812500000000007</v>
+        <v>0.1316725978647687</v>
       </c>
       <c r="C4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>APG1L</t>
+          <t>ARC1T</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.07803468208092486</v>
+        <v>0.05454545454545439</v>
       </c>
       <c r="C5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RJR1R</t>
+          <t>IVL1L</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.07142857142857133</v>
+        <v>0.03603603603603607</v>
       </c>
       <c r="C6" s="1" t="n"/>
     </row>
@@ -1120,55 +1120,55 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SMA1R</t>
+          <t>TSM1T</t>
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>-0.4545454545454545</v>
+        <v>-0.0651162790697675</v>
       </c>
       <c r="C8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>RAR1R</t>
+          <t>SFG1T</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>-0.3176470588235295</v>
+        <v>-0.04888888888888884</v>
       </c>
       <c r="C9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RKB1R</t>
+          <t>EWA1L</t>
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>-0.1219512195121949</v>
+        <v>-0.0451612903225806</v>
       </c>
       <c r="C10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BLT1T</t>
+          <t>NTU1L</t>
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>-0.09243697478991593</v>
+        <v>-0.03749999999999998</v>
       </c>
       <c r="C11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AMG1L</t>
+          <t>SAF1R</t>
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>-0.09166666666666656</v>
+        <v>-0.03067484662576676</v>
       </c>
       <c r="C12" s="1" t="n"/>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2019.04.12</t>
+          <t>2019.05.31</t>
         </is>
       </c>
     </row>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2019.04.05</t>
+          <t>2019.05.24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
-updated xlsx template, -expanded print area -removed old temp files from repo. -added sample output png from recent run
</commit_message>
<xml_diff>
--- a/data/Template.xlsx
+++ b/data/Template.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Output_Area">Main!$D$1:$R$18</definedName>
+    <definedName name="Output_Area">Main!$D$1:$R$25</definedName>
   </definedNames>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
@@ -20,7 +20,7 @@
   <numFmts count="1">
     <numFmt formatCode="0.0%" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="186"/>
@@ -62,6 +62,21 @@
       <color theme="1"/>
       <sz val="14"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="186"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="186"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -84,7 +99,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -94,6 +109,11 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -223,7 +243,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t>None</a:t>
+                  <a:t/>
                 </a:r>
                 <a:endParaRPr lang="lt-LT"/>
               </a:p>
@@ -242,19 +262,19 @@
               <strCache>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>TSM1T</v>
+                  <v>GRZ1R</v>
                 </pt>
                 <pt idx="1">
-                  <v>SFG1T</v>
+                  <v>SKN1T</v>
                 </pt>
                 <pt idx="2">
-                  <v>EWA1L</v>
+                  <v>INL1L</v>
                 </pt>
                 <pt idx="3">
-                  <v>NTU1L</v>
+                  <v>SNG1L</v>
                 </pt>
                 <pt idx="4">
-                  <v>SAF1R</v>
+                  <v>PKG1T</v>
                 </pt>
               </strCache>
             </strRef>
@@ -266,19 +286,19 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>-0.05</v>
+                  <v>-0.5212765957446808</v>
                 </pt>
                 <pt idx="1">
-                  <v>-0.05</v>
+                  <v>-0.177570093457944</v>
                 </pt>
                 <pt idx="2">
-                  <v>-0.05</v>
+                  <v>-0.135678391959799</v>
                 </pt>
                 <pt idx="3">
-                  <v>-0.05</v>
+                  <v>-0.0789473684210527</v>
                 </pt>
                 <pt idx="4">
-                  <v>-0.05</v>
+                  <v>-0.07586206896551716</v>
                 </pt>
               </numCache>
             </numRef>
@@ -293,11 +313,11 @@
           <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="100"/>
-        <axId val="110719600"/>
-        <axId val="110720160"/>
+        <axId val="4996544"/>
+        <axId val="207576752"/>
       </barChart>
       <catAx>
-        <axId val="110719600"/>
+        <axId val="4996544"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -338,12 +358,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="110720160"/>
+        <crossAx val="207576752"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -351,7 +371,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="110720160"/>
+        <axId val="207576752"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -386,12 +406,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="110719600"/>
+        <crossAx val="4996544"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -522,7 +542,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t>None</a:t>
+                  <a:t/>
                 </a:r>
                 <a:endParaRPr lang="lt-LT"/>
               </a:p>
@@ -541,19 +561,19 @@
               <strCache>
                 <ptCount val="5"/>
                 <pt idx="0">
+                  <v>LJM1R</v>
+                </pt>
+                <pt idx="1">
+                  <v>GRD1R</v>
+                </pt>
+                <pt idx="2">
                   <v>RKB1R</v>
                 </pt>
-                <pt idx="1">
-                  <v>SKN1T</v>
-                </pt>
-                <pt idx="2">
-                  <v>OLF1R</v>
-                </pt>
                 <pt idx="3">
-                  <v>ARC1T</v>
+                  <v>BLT1T</v>
                 </pt>
                 <pt idx="4">
-                  <v>IVL1L</v>
+                  <v>RJR1R</v>
                 </pt>
               </strCache>
             </strRef>
@@ -565,19 +585,19 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>0.05</v>
+                  <v>0.2</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.05</v>
+                  <v>0.1607142857142858</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.05</v>
+                  <v>0.1111111111111111</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.05</v>
+                  <v>0.08787878787878778</v>
                 </pt>
                 <pt idx="4">
-                  <v>0.05</v>
+                  <v>0.07647058823529401</v>
                 </pt>
               </numCache>
             </numRef>
@@ -592,11 +612,11 @@
           <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="100"/>
-        <axId val="183703744"/>
-        <axId val="183704304"/>
+        <axId val="207578992"/>
+        <axId val="207579552"/>
       </barChart>
       <catAx>
-        <axId val="183703744"/>
+        <axId val="207578992"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -637,12 +657,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="183704304"/>
+        <crossAx val="207579552"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -650,7 +670,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="183704304"/>
+        <axId val="207579552"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -685,12 +705,529 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="183703744"/>
+        <crossAx val="207578992"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <strRef>
+          <f>Main!$K$18</f>
+          <strCache>
+            <ptCount val="1"/>
+            <pt idx="0">
+              <v>Random metric for the week: D&amp;A/Total Assets</v>
+            </pt>
+          </strCache>
+        </strRef>
+      </tx>
+      <layout/>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+      <txPr>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr>
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr lang="lt-LT"/>
+        </a:p>
+      </txPr>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>Main!$A$21</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>D&amp;A/Total Assets</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>Main!$I$20:$I$24</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Baltika</v>
+                </pt>
+                <pt idx="1">
+                  <v>Grigeo Grigiškės</v>
+                </pt>
+                <pt idx="2">
+                  <v>Telia Lietuva</v>
+                </pt>
+                <pt idx="3">
+                  <v>Linda Nektar</v>
+                </pt>
+                <pt idx="4">
+                  <v>Pieno žvaigždės</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>Main!$V$24:$V$28</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.1171057019006335</v>
+                </pt>
+                <pt idx="1">
+                  <v>0.1157838350991999</v>
+                </pt>
+                <pt idx="2">
+                  <v>0.1141666888256619</v>
+                </pt>
+                <pt idx="3">
+                  <v>0.1134136904799231</v>
+                </pt>
+                <pt idx="4">
+                  <v>0.09259561725874507</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="219"/>
+        <overlap val="-27"/>
+        <axId val="872368768"/>
+        <axId val="872369888"/>
+      </barChart>
+      <catAx>
+        <axId val="872368768"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="lt-LT"/>
+          </a:p>
+        </txPr>
+        <crossAx val="872369888"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="872369888"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="lt-LT"/>
+          </a:p>
+        </txPr>
+        <crossAx val="872368768"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:r>
+              <a:t/>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <layout/>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+      <txPr>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr>
+            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:t/>
+          </a:r>
+          <a:endParaRPr lang="lt-LT"/>
+        </a:p>
+      </txPr>
+    </title>
+    <plotArea>
+      <layout/>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>Main!$A$21</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>D&amp;A/Total Assets</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>Main!$A$110:$A$114</f>
+              <strCache>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>Baltika</v>
+                </pt>
+                <pt idx="1">
+                  <v>Grigeo Grigiškės</v>
+                </pt>
+                <pt idx="2">
+                  <v>Telia Lietuva</v>
+                </pt>
+                <pt idx="3">
+                  <v>Linda Nektar</v>
+                </pt>
+                <pt idx="4">
+                  <v>Pieno žvaigždės</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>Main!$E$110:$E$114</f>
+              <numCache>
+                <formatCode>0.00%</formatCode>
+                <ptCount val="5"/>
+                <pt idx="0">
+                  <v>0.1171</v>
+                </pt>
+                <pt idx="1">
+                  <v>0.1158</v>
+                </pt>
+                <pt idx="2">
+                  <v>0.1142</v>
+                </pt>
+                <pt idx="3">
+                  <v>0.1134</v>
+                </pt>
+                <pt idx="4">
+                  <v>0.0926</v>
+                </pt>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+        </dLbls>
+        <gapWidth val="219"/>
+        <overlap val="-27"/>
+        <axId val="282785328"/>
+        <axId val="282784768"/>
+      </barChart>
+      <catAx>
+        <axId val="282785328"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="800">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="lt-LT"/>
+          </a:p>
+        </txPr>
+        <crossAx val="282784768"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="282784768"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="0.00%" sourceLinked="1"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t/>
+            </a:r>
+            <a:endParaRPr lang="lt-LT"/>
+          </a:p>
+        </txPr>
+        <crossAx val="282785328"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -752,6 +1289,60 @@
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>428625</colOff>
+      <row>26</row>
+      <rowOff>138112</rowOff>
+    </from>
+    <to>
+      <col>14</col>
+      <colOff>123825</colOff>
+      <row>41</row>
+      <rowOff>23812</rowOff>
+    </to>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>238125</colOff>
+      <row>98</row>
+      <rowOff>52387</rowOff>
+    </from>
+    <to>
+      <col>12</col>
+      <colOff>542925</colOff>
+      <row>112</row>
+      <rowOff>128587</rowOff>
+    </to>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1027,14 +1618,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:V114"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="28"/>
     <col customWidth="1" max="4" min="4" width="2.7109375"/>
     <col customWidth="1" max="18" min="18" width="2.7109375"/>
   </cols>
@@ -1051,25 +1643,25 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row customHeight="1" ht="7.5" r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>RKB1R</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>0.1969696969696969</v>
+        <v>0.212121212121212</v>
       </c>
       <c r="C2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SKN1T</t>
+          <t>GRD1R</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0.153846153846154</v>
+        <v>0.1944444444444444</v>
       </c>
       <c r="C3" s="1" t="n"/>
       <c r="K3" s="3">
@@ -1080,33 +1672,33 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>OLF1R</t>
+          <t>LJM1R</t>
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.1316725978647687</v>
+        <v>0.06666666666666662</v>
       </c>
       <c r="C4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ARC1T</t>
+          <t>OLF1R</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.05454545454545439</v>
+        <v>0.05120481927710855</v>
       </c>
       <c r="C5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IVL1L</t>
+          <t>SAB1L</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.03603603603603607</v>
+        <v>0.0492505353319057</v>
       </c>
       <c r="C6" s="1" t="n"/>
     </row>
@@ -1120,59 +1712,60 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TSM1T</t>
+          <t>BLT1T</t>
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>-0.0651162790697675</v>
+        <v>-0.3125</v>
       </c>
       <c r="C8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SFG1T</t>
+          <t>INL1L</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>-0.04888888888888884</v>
+        <v>-0.135678391959799</v>
       </c>
       <c r="C9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EWA1L</t>
+          <t>SNG1L</t>
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>-0.0451612903225806</v>
+        <v>-0.0789473684210527</v>
       </c>
       <c r="C10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NTU1L</t>
+          <t>K2LT</t>
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>-0.03749999999999998</v>
+        <v>-0.06060606060606061</v>
       </c>
       <c r="C11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SAF1R</t>
+          <t>RJR1R</t>
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>-0.03067484662576676</v>
+        <v>-0.05670103092783497</v>
       </c>
       <c r="C12" s="1" t="n"/>
     </row>
-    <row r="18">
+    <row customHeight="1" ht="7.5" r="17"/>
+    <row customHeight="1" ht="15.75" r="18">
       <c r="A18" t="inlineStr">
         <is>
           <t>Start date</t>
@@ -1180,11 +1773,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2019.05.31</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
+          <t>2019.07.23</t>
+        </is>
+      </c>
+      <c r="K18" s="5">
+        <f>"Random metric for the week: "&amp;$A$21</f>
+        <v/>
+      </c>
+    </row>
+    <row customHeight="1" ht="9" r="19">
       <c r="A19" t="inlineStr">
         <is>
           <t>End date</t>
@@ -1192,8 +1789,849 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2019.05.24</t>
-        </is>
+          <t>2019.07.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Used format</t>
+        </is>
+      </c>
+      <c r="I20">
+        <f>U24</f>
+        <v/>
+      </c>
+      <c r="M20">
+        <f>TEXT(V24,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Adj. Net profit margin</t>
+        </is>
+      </c>
+      <c r="B21" s="6">
+        <f>INDEX($B$30:$B$64,MATCH($A$21,$A$30:$A$64,0))</f>
+        <v/>
+      </c>
+      <c r="I21">
+        <f>U25</f>
+        <v/>
+      </c>
+      <c r="M21">
+        <f>TEXT(V25,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="I22">
+        <f>U26</f>
+        <v/>
+      </c>
+      <c r="M22">
+        <f>TEXT(V26,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="I23">
+        <f>U27</f>
+        <v/>
+      </c>
+      <c r="M23">
+        <f>TEXT(V27,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>All types</t>
+        </is>
+      </c>
+      <c r="I24">
+        <f>U28</f>
+        <v/>
+      </c>
+      <c r="M24">
+        <f>TEXT(V28,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
+        <v/>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>Invalda INVL</t>
+        </is>
+      </c>
+      <c r="V24" t="n">
+        <v>1.055735056542811</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>Tallinna Vesi</t>
+        </is>
+      </c>
+      <c r="V25" t="n">
+        <v>0.3846766486142084</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>Amber Grid</t>
+        </is>
+      </c>
+      <c r="V26" t="n">
+        <v>0.2964450174986185</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>INVL Baltic Real Estate</t>
+        </is>
+      </c>
+      <c r="V27" t="n">
+        <v>0.2913088285812436</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>INVL Baltic Farmland</t>
+        </is>
+      </c>
+      <c r="V28" t="n">
+        <v>0.2389937106918239</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>Ratio</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>Format</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Market Cap., k €</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>EV, k €</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>TOTAL ASSETS</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Book value</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Tangible Book Value</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Minority/Equity</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Intangibles/Equity</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ROA</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Inventory</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Total Receivables</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>D&amp;A/Total Assets</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>D&amp;A/Fixed assets</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>EV/EBITDA</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>EV/EBITDA adj.</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>P/E</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>P/E adj.</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>P/tBV</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>NNWC/Market Cap</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Debt/Equity</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Financial debt/Total liabilities</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Net Debt/EBITDA adj.</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Current Ratio</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Quick Ratio</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Gross profit margin</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Operating profit margin</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Adj. Net profit margin</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Adj. EBITDA margin</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Cash/Assets</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Retained earnings/Assets</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Cash/Retained Earnings</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Cash/Market Cap</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>FCF/Market Cap</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Dividend yield</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Payout ratio</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Size</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Balance Ratios</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Valuation</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Liquidity</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Margins</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Dividend Potential</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Market Cap., k €</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Book value</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>EV/EBITDA</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Debt/Equity</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Gross profit margin</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Cash/Assets</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>EV, k €</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Tangible Book Value</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>EV/EBITDA adj.</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>Financial debt/Total liabilities</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Operating profit margin</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>Retained earnings/Assets</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>TOTAL ASSETS</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Minority/Equity</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>P/E</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Net Debt/EBITDA adj.</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Adj. Net profit margin</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Cash/Retained Earnings</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Intangibles/Equity</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>P/E adj.</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Current Ratio</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Adj. EBITDA margin</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>Cash/Market Cap</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>P/tBV</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Quick Ratio</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>FCF/Market Cap</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>ROA</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>NNWC/Market Cap</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Dividend yield</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Inventory</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Payout ratio</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Total Receivables</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>D&amp;A/Total Assets</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>D&amp;A/Fixed assets</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Baltika</t>
+        </is>
+      </c>
+      <c r="E110" s="7" t="n">
+        <v>0.1171</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Grigeo Grigiškės</t>
+        </is>
+      </c>
+      <c r="E111" s="7" t="n">
+        <v>0.1158</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Telia Lietuva</t>
+        </is>
+      </c>
+      <c r="E112" s="7" t="n">
+        <v>0.1142</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Linda Nektar</t>
+        </is>
+      </c>
+      <c r="E113" s="7" t="n">
+        <v>0.1134</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Pieno žvaigždės</t>
+        </is>
+      </c>
+      <c r="E114" s="7" t="n">
+        <v>0.0926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed template.xlsx -added third chart to display ratios visually -edited vba macro to remove outline on third chart -vba script also changes axis number format -updated output example png -edited report_generator.py docstring
</commit_message>
<xml_diff>
--- a/data/Template.xlsx
+++ b/data/Template.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Output_Area">Main!$D$1:$R$25</definedName>
+    <definedName name="Output_Area">Main!$D$1:$R$31</definedName>
   </definedNames>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
@@ -262,19 +262,19 @@
               <strCache>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>GRZ1R</v>
+                  <v>BLT1T</v>
                 </pt>
                 <pt idx="1">
-                  <v>SKN1T</v>
+                  <v>INL1L</v>
                 </pt>
                 <pt idx="2">
-                  <v>INL1L</v>
+                  <v>SNG1L</v>
                 </pt>
                 <pt idx="3">
-                  <v>SNG1L</v>
+                  <v>K2LT</v>
                 </pt>
                 <pt idx="4">
-                  <v>PKG1T</v>
+                  <v>RJR1R</v>
                 </pt>
               </strCache>
             </strRef>
@@ -286,19 +286,19 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>-0.5212765957446808</v>
+                  <v>-0.3125</v>
                 </pt>
                 <pt idx="1">
-                  <v>-0.177570093457944</v>
+                  <v>-0.135678391959799</v>
                 </pt>
                 <pt idx="2">
-                  <v>-0.135678391959799</v>
+                  <v>-0.0789473684210527</v>
                 </pt>
                 <pt idx="3">
-                  <v>-0.0789473684210527</v>
+                  <v>-0.06060606060606061</v>
                 </pt>
                 <pt idx="4">
-                  <v>-0.07586206896551716</v>
+                  <v>-0.05670103092783497</v>
                 </pt>
               </numCache>
             </numRef>
@@ -313,11 +313,11 @@
           <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="100"/>
-        <axId val="4996544"/>
-        <axId val="207576752"/>
+        <axId val="38426464"/>
+        <axId val="38427024"/>
       </barChart>
       <catAx>
-        <axId val="4996544"/>
+        <axId val="38426464"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -347,10 +347,7 @@
             <a:pPr>
               <a:defRPr b="1" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr lastClr="000000" val="windowText"/>
                 </a:solidFill>
                 <a:latin charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
                 <a:ea typeface="+mn-ea"/>
@@ -363,7 +360,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="207576752"/>
+        <crossAx val="38427024"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -371,7 +368,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="207576752"/>
+        <axId val="38427024"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -411,7 +408,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="4996544"/>
+        <crossAx val="38426464"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -561,19 +558,19 @@
               <strCache>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>LJM1R</v>
+                  <v>RKB1R</v>
                 </pt>
                 <pt idx="1">
                   <v>GRD1R</v>
                 </pt>
                 <pt idx="2">
-                  <v>RKB1R</v>
+                  <v>LJM1R</v>
                 </pt>
                 <pt idx="3">
-                  <v>BLT1T</v>
+                  <v>OLF1R</v>
                 </pt>
                 <pt idx="4">
-                  <v>RJR1R</v>
+                  <v>SAB1L</v>
                 </pt>
               </strCache>
             </strRef>
@@ -585,19 +582,19 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>0.2</v>
+                  <v>0.212121212121212</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.1607142857142858</v>
+                  <v>0.1944444444444444</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.1111111111111111</v>
+                  <v>0.06666666666666662</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.08787878787878778</v>
+                  <v>0.05120481927710855</v>
                 </pt>
                 <pt idx="4">
-                  <v>0.07647058823529401</v>
+                  <v>0.0492505353319057</v>
                 </pt>
               </numCache>
             </numRef>
@@ -612,11 +609,11 @@
           <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="100"/>
-        <axId val="207578992"/>
-        <axId val="207579552"/>
+        <axId val="202097200"/>
+        <axId val="202097760"/>
       </barChart>
       <catAx>
-        <axId val="207578992"/>
+        <axId val="202097200"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -646,10 +643,7 @@
             <a:pPr>
               <a:defRPr b="1" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr lastClr="000000" val="windowText"/>
                 </a:solidFill>
                 <a:latin charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
                 <a:ea typeface="+mn-ea"/>
@@ -662,7 +656,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="207579552"/>
+        <crossAx val="202097760"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -670,7 +664,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="207579552"/>
+        <axId val="202097760"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -710,7 +704,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="207578992"/>
+        <crossAx val="202097200"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -727,11 +721,11 @@
     <title>
       <tx>
         <strRef>
-          <f>Main!$K$18</f>
+          <f>Main!$K$40</f>
           <strCache>
             <ptCount val="1"/>
             <pt idx="0">
-              <v>Random metric for the week: D&amp;A/Total Assets</v>
+              <v>Random metric for the week: TOTAL ASSETS</v>
             </pt>
           </strCache>
         </strRef>
@@ -750,16 +744,13 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
-            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
+            <a:defRPr b="1" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1100">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr lastClr="000000" val="windowText"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
           <a:r>
@@ -770,7 +761,19 @@
       </txPr>
     </title>
     <plotArea>
-      <layout/>
+      <layout>
+        <manualLayout>
+          <layoutTarget val="inner"/>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.07132468175456302"/>
+          <y val="0.1348709405081727"/>
+          <w val="0.8770832182857433"/>
+          <h val="0.7392793731105993"/>
+        </manualLayout>
+      </layout>
       <barChart>
         <barDir val="col"/>
         <grouping val="clustered"/>
@@ -784,14 +787,14 @@
               <strCache>
                 <ptCount val="1"/>
                 <pt idx="0">
-                  <v>D&amp;A/Total Assets</v>
+                  <v>TOTAL ASSETS</v>
                 </pt>
               </strCache>
             </strRef>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="245D90"/>
             </a:solidFill>
             <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:noFill/>
@@ -801,23 +804,23 @@
           <invertIfNegative val="0"/>
           <cat>
             <strRef>
-              <f>Main!$I$20:$I$24</f>
+              <f>Main!$I$43:$I$47</f>
               <strCache>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>Baltika</v>
+                  <v>Siguldas CMAS</v>
                 </pt>
                 <pt idx="1">
-                  <v>Grigeo Grigiškės</v>
+                  <v>K2 LT</v>
                 </pt>
                 <pt idx="2">
-                  <v>Telia Lietuva</v>
+                  <v>Linda Nektar</v>
                 </pt>
                 <pt idx="3">
-                  <v>Linda Nektar</v>
+                  <v>Ditton pievadķēžu rūpnīca</v>
                 </pt>
                 <pt idx="4">
-                  <v>Pieno žvaigždės</v>
+                  <v>MADARA Cosmetics</v>
                 </pt>
               </strCache>
             </strRef>
@@ -829,19 +832,19 @@
                 <formatCode>General</formatCode>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>0.1171057019006335</v>
+                  <v>1572.482</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.1157838350991999</v>
+                  <v>2752.856</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.1141666888256619</v>
+                  <v>3986.785</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.1134136904799231</v>
+                  <v>8816.085999999999</v>
                 </pt>
                 <pt idx="4">
-                  <v>0.09259561725874507</v>
+                  <v>9845.353999999999</v>
                 </pt>
               </numCache>
             </numRef>
@@ -855,13 +858,13 @@
           <showPercent val="0"/>
           <showBubbleSize val="0"/>
         </dLbls>
-        <gapWidth val="219"/>
+        <gapWidth val="88"/>
         <overlap val="-27"/>
-        <axId val="872368768"/>
-        <axId val="872369888"/>
+        <axId val="202100000"/>
+        <axId val="202100560"/>
       </barChart>
       <catAx>
-        <axId val="872368768"/>
+        <axId val="202100000"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -889,16 +892,13 @@
           <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
-              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
+              <a:defRPr b="1" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr lastClr="000000" val="windowText"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -907,7 +907,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="872369888"/>
+        <crossAx val="202100560"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -915,7 +915,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="872369888"/>
+        <axId val="202100560"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -923,15 +923,14 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="9525">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="6350">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="62000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:prstDash val="solid"/>
-              <a:round/>
+              <a:miter lim="800000"/>
             </a:ln>
           </spPr>
         </majorGridlines>
@@ -969,7 +968,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="872368768"/>
+        <crossAx val="202100000"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -987,14 +986,15 @@
       <tx>
         <rich>
           <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
           <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:r>
               <a:t/>
             </a:r>
+            <a:endParaRPr/>
           </a:p>
         </rich>
       </tx>
-      <layout/>
       <overlay val="0"/>
       <spPr>
         <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
@@ -1003,29 +1003,6 @@
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
-      <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr>
-            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:t/>
-          </a:r>
-          <a:endParaRPr lang="lt-LT"/>
-        </a:p>
-      </txPr>
     </title>
     <plotArea>
       <layout/>
@@ -1042,7 +1019,7 @@
               <strCache>
                 <ptCount val="1"/>
                 <pt idx="0">
-                  <v>D&amp;A/Total Assets</v>
+                  <v>TOTAL ASSETS</v>
                 </pt>
               </strCache>
             </strRef>
@@ -1115,11 +1092,11 @@
         </dLbls>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="282785328"/>
-        <axId val="282784768"/>
+        <axId val="202102800"/>
+        <axId val="202103360"/>
       </barChart>
       <catAx>
-        <axId val="282785328"/>
+        <axId val="202102800"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1165,7 +1142,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="282784768"/>
+        <crossAx val="202103360"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1173,7 +1150,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="282784768"/>
+        <axId val="202103360"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1227,7 +1204,7 @@
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="282785328"/>
+        <crossAx val="202102800"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -1296,16 +1273,16 @@
   </twoCellAnchor>
   <twoCellAnchor>
     <from>
-      <col>6</col>
-      <colOff>428625</colOff>
-      <row>26</row>
-      <rowOff>138112</rowOff>
+      <col>4</col>
+      <colOff>28574</colOff>
+      <row>16</row>
+      <rowOff>71437</rowOff>
     </from>
     <to>
-      <col>14</col>
-      <colOff>123825</colOff>
-      <row>41</row>
-      <rowOff>23812</rowOff>
+      <col>16</col>
+      <colOff>590549</colOff>
+      <row>31</row>
+      <rowOff>57150</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1643,7 +1620,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="7.5" r="2">
+    <row customHeight="1" ht="6.75" r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>RKB1R</t>
@@ -1669,7 +1646,7 @@
         <v/>
       </c>
     </row>
-    <row r="4">
+    <row customHeight="1" ht="9.75" r="4">
       <c r="A4" t="inlineStr">
         <is>
           <t>LJM1R</t>
@@ -1776,12 +1753,8 @@
           <t>2019.07.23</t>
         </is>
       </c>
-      <c r="K18" s="5">
-        <f>"Random metric for the week: "&amp;$A$21</f>
-        <v/>
-      </c>
-    </row>
-    <row customHeight="1" ht="9" r="19">
+    </row>
+    <row r="19">
       <c r="A19" t="inlineStr">
         <is>
           <t>End date</t>
@@ -1799,358 +1772,358 @@
           <t>Used format</t>
         </is>
       </c>
-      <c r="I20">
-        <f>U24</f>
-        <v/>
-      </c>
-      <c r="M20">
-        <f>TEXT(V24,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Adj. Net profit margin</t>
+          <t>P/tBV</t>
         </is>
       </c>
       <c r="B21" s="6">
         <f>INDEX($B$30:$B$64,MATCH($A$21,$A$30:$A$64,0))</f>
         <v/>
       </c>
-      <c r="I21">
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>All types</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>Baltika</t>
+        </is>
+      </c>
+      <c r="V24" t="n">
+        <v>-0.3752931242532856</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>Panevėžio statybos trestas</t>
+        </is>
+      </c>
+      <c r="V25" t="n">
+        <v>0.3405392938018955</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>Kauno energija</t>
+        </is>
+      </c>
+      <c r="V26" t="n">
+        <v>0.4568353691700483</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>Linas Agro Group</t>
+        </is>
+      </c>
+      <c r="V27" t="n">
+        <v>0.5806016885843802</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>Valmieras stikla šķiedra</t>
+        </is>
+      </c>
+      <c r="V28" t="n">
+        <v>0.6312485621461308</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>Ratio</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>Format</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Market Cap., k €</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>EV, k €</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>TOTAL ASSETS</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Book value</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Tangible Book Value</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Minority/Equity</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Intangibles/Equity</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ROE</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ROA</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Inventory</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Total Receivables</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="K40" s="5">
+        <f>"Random metric for the week: "&amp;$A$21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>D&amp;A/Total Assets</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>D&amp;A/Fixed assets</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>EV/EBITDA</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="I43">
+        <f>U24</f>
+        <v/>
+      </c>
+      <c r="M43">
+        <f>TEXT(V24,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>EV/EBITDA adj.</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="I44">
         <f>U25</f>
         <v/>
       </c>
-      <c r="M21">
+      <c r="M44">
         <f>TEXT(V25,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
         <v/>
       </c>
     </row>
-    <row r="22">
-      <c r="I22">
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>P/E</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="I45">
         <f>U26</f>
         <v/>
       </c>
-      <c r="M22">
+      <c r="M45">
         <f>TEXT(V26,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
         <v/>
       </c>
     </row>
-    <row r="23">
-      <c r="I23">
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>P/E adj.</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="I46">
         <f>U27</f>
         <v/>
       </c>
-      <c r="M23">
+      <c r="M46">
         <f>TEXT(V27,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
         <v/>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>All types</t>
-        </is>
-      </c>
-      <c r="I24">
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>P/tBV</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="I47">
         <f>U28</f>
         <v/>
       </c>
-      <c r="M24">
+      <c r="M47">
         <f>TEXT(V28,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
         <v/>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>Invalda INVL</t>
-        </is>
-      </c>
-      <c r="V24" t="n">
-        <v>1.055735056542811</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>Tallinna Vesi</t>
-        </is>
-      </c>
-      <c r="V25" t="n">
-        <v>0.3846766486142084</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>Amber Grid</t>
-        </is>
-      </c>
-      <c r="V26" t="n">
-        <v>0.2964450174986185</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>INVL Baltic Real Estate</t>
-        </is>
-      </c>
-      <c r="V27" t="n">
-        <v>0.2913088285812436</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>INVL Baltic Farmland</t>
-        </is>
-      </c>
-      <c r="V28" t="n">
-        <v>0.2389937106918239</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>Ratio</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>Format</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Market Cap., k €</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>EV, k €</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>TOTAL ASSETS</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Book value</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Tangible Book Value</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Minority/Equity</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Intangibles/Equity</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>ROE</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>ROA</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Inventory</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Total Receivables</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>D&amp;A/Total Assets</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>D&amp;A/Fixed assets</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>EV/EBITDA</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>EV/EBITDA adj.</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>P/E</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>P/E adj.</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>P/tBV</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
       </c>
     </row>
     <row r="48">

</xml_diff>

<commit_message>
-Improved output graph semantics -screener_handler.py now outputs additional arg: random_bool -which is passed to template.xlsx to form more precise description -removed missed commented line -added another png example of current output
</commit_message>
<xml_diff>
--- a/data/Template.xlsx
+++ b/data/Template.xlsx
@@ -20,7 +20,7 @@
   <numFmts count="1">
     <numFmt formatCode="0.0%" numFmtId="164"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <charset val="186"/>
@@ -77,13 +77,27 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="186"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,7 +113,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -113,7 +127,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -243,7 +259,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="lt-LT"/>
               </a:p>
@@ -265,16 +281,16 @@
                   <v>BLT1T</v>
                 </pt>
                 <pt idx="1">
-                  <v>INL1L</v>
+                  <v>SAF1R</v>
                 </pt>
                 <pt idx="2">
-                  <v>SNG1L</v>
+                  <v>TVEAT</v>
                 </pt>
                 <pt idx="3">
-                  <v>K2LT</v>
+                  <v>SMA1R</v>
                 </pt>
                 <pt idx="4">
-                  <v>RJR1R</v>
+                  <v>HAE1T</v>
                 </pt>
               </strCache>
             </strRef>
@@ -286,19 +302,19 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>-0.3125</v>
+                  <v>-0.3314763231197771</v>
                 </pt>
                 <pt idx="1">
-                  <v>-0.135678391959799</v>
+                  <v>-0.04761904761904766</v>
                 </pt>
                 <pt idx="2">
-                  <v>-0.0789473684210527</v>
+                  <v>-0.03508771929824565</v>
                 </pt>
                 <pt idx="3">
-                  <v>-0.06060606060606061</v>
+                  <v>-0.02702702702702703</v>
                 </pt>
                 <pt idx="4">
-                  <v>-0.05670103092783497</v>
+                  <v>-0.0263736263736264</v>
                 </pt>
               </numCache>
             </numRef>
@@ -313,11 +329,11 @@
           <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="100"/>
-        <axId val="38426464"/>
-        <axId val="38427024"/>
+        <axId val="179616240"/>
+        <axId val="179616800"/>
       </barChart>
       <catAx>
-        <axId val="38426464"/>
+        <axId val="179616240"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -355,12 +371,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="38427024"/>
+        <crossAx val="179616800"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -368,7 +384,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="38427024"/>
+        <axId val="179616800"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -403,12 +419,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="38426464"/>
+        <crossAx val="179616240"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -539,7 +555,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
                 <a:endParaRPr lang="lt-LT"/>
               </a:p>
@@ -561,16 +577,16 @@
                   <v>RKB1R</v>
                 </pt>
                 <pt idx="1">
-                  <v>GRD1R</v>
+                  <v>SKN1T</v>
                 </pt>
                 <pt idx="2">
-                  <v>LJM1R</v>
+                  <v>PKG1T</v>
                 </pt>
                 <pt idx="3">
-                  <v>OLF1R</v>
+                  <v>SAB1L</v>
                 </pt>
                 <pt idx="4">
-                  <v>SAB1L</v>
+                  <v>UTR1L</v>
                 </pt>
               </strCache>
             </strRef>
@@ -582,19 +598,19 @@
                 <formatCode>0.0%</formatCode>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>0.212121212121212</v>
+                  <v>0.3000000000000002</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.1944444444444444</v>
+                  <v>0.09090909090909087</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.06666666666666662</v>
+                  <v>0.08208955223880587</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.05120481927710855</v>
+                  <v>0.05543710021321967</v>
                 </pt>
                 <pt idx="4">
-                  <v>0.0492505353319057</v>
+                  <v>0.05000000000000004</v>
                 </pt>
               </numCache>
             </numRef>
@@ -609,11 +625,11 @@
           <showBubbleSize val="0"/>
         </dLbls>
         <gapWidth val="100"/>
-        <axId val="202097200"/>
-        <axId val="202097760"/>
+        <axId val="179619040"/>
+        <axId val="220759904"/>
       </barChart>
       <catAx>
-        <axId val="202097200"/>
+        <axId val="179619040"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -651,12 +667,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="202097760"/>
+        <crossAx val="220759904"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -664,7 +680,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="202097760"/>
+        <axId val="220759904"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -699,12 +715,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="202097200"/>
+        <crossAx val="179619040"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -721,11 +737,11 @@
     <title>
       <tx>
         <strRef>
-          <f>Main!$K$40</f>
+          <f>Main!$Q$40</f>
           <strCache>
             <ptCount val="1"/>
             <pt idx="0">
-              <v>Random metric for the week: TOTAL ASSETS</v>
+              <v>Balance Structure: Highest Accumulated Retained Earnings in Total Assets</v>
             </pt>
           </strCache>
         </strRef>
@@ -754,7 +770,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="lt-LT"/>
         </a:p>
@@ -787,7 +803,7 @@
               <strCache>
                 <ptCount val="1"/>
                 <pt idx="0">
-                  <v>TOTAL ASSETS</v>
+                  <v>Retained earnings/Assets</v>
                 </pt>
               </strCache>
             </strRef>
@@ -804,23 +820,23 @@
           <invertIfNegative val="0"/>
           <cat>
             <strRef>
-              <f>Main!$I$43:$I$47</f>
+              <f>Main!$O$43:$O$47</f>
               <strCache>
                 <ptCount val="5"/>
                 <pt idx="0">
+                  <v>Invalda INVL</v>
+                </pt>
+                <pt idx="1">
+                  <v>Silvano Fashion Group</v>
+                </pt>
+                <pt idx="2">
                   <v>Siguldas CMAS</v>
                 </pt>
-                <pt idx="1">
-                  <v>K2 LT</v>
-                </pt>
-                <pt idx="2">
-                  <v>Linda Nektar</v>
-                </pt>
                 <pt idx="3">
-                  <v>Ditton pievadķēžu rūpnīca</v>
+                  <v>Olainfarm</v>
                 </pt>
                 <pt idx="4">
-                  <v>MADARA Cosmetics</v>
+                  <v>Harju Elekter</v>
                 </pt>
               </strCache>
             </strRef>
@@ -832,19 +848,19 @@
                 <formatCode>General</formatCode>
                 <ptCount val="5"/>
                 <pt idx="0">
-                  <v>1572.482</v>
+                  <v>0.6638684854844351</v>
                 </pt>
                 <pt idx="1">
-                  <v>2752.856</v>
+                  <v>0.6225826300984529</v>
                 </pt>
                 <pt idx="2">
-                  <v>3986.785</v>
+                  <v>0.5680987127356625</v>
                 </pt>
                 <pt idx="3">
-                  <v>8816.085999999999</v>
+                  <v>0.5616823630426405</v>
                 </pt>
                 <pt idx="4">
-                  <v>9845.353999999999</v>
+                  <v>0.5330045948671971</v>
                 </pt>
               </numCache>
             </numRef>
@@ -860,11 +876,11 @@
         </dLbls>
         <gapWidth val="88"/>
         <overlap val="-27"/>
-        <axId val="202100000"/>
-        <axId val="202100560"/>
+        <axId val="220762144"/>
+        <axId val="220762704"/>
       </barChart>
       <catAx>
-        <axId val="202100000"/>
+        <axId val="220762144"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -873,7 +889,7 @@
         <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
+        <tickLblPos val="low"/>
         <spPr>
           <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
           <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="9525">
@@ -902,12 +918,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="202100560"/>
+        <crossAx val="220762704"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -915,7 +931,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="202100560"/>
+        <axId val="220762704"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -963,248 +979,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="lt-LT"/>
           </a:p>
         </txPr>
-        <crossAx val="202100000"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="between"/>
-      </valAx>
-    </plotArea>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:r>
-              <a:t/>
-            </a:r>
-            <a:endParaRPr/>
-          </a:p>
-        </rich>
-      </tx>
-      <overlay val="0"/>
-      <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </title>
-    <plotArea>
-      <layout/>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <varyColors val="0"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>Main!$A$21</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>TOTAL ASSETS</v>
-                </pt>
-              </strCache>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <invertIfNegative val="0"/>
-          <cat>
-            <strRef>
-              <f>Main!$A$110:$A$114</f>
-              <strCache>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>Baltika</v>
-                </pt>
-                <pt idx="1">
-                  <v>Grigeo Grigiškės</v>
-                </pt>
-                <pt idx="2">
-                  <v>Telia Lietuva</v>
-                </pt>
-                <pt idx="3">
-                  <v>Linda Nektar</v>
-                </pt>
-                <pt idx="4">
-                  <v>Pieno žvaigždės</v>
-                </pt>
-              </strCache>
-            </strRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>Main!$E$110:$E$114</f>
-              <numCache>
-                <formatCode>0.00%</formatCode>
-                <ptCount val="5"/>
-                <pt idx="0">
-                  <v>0.1171</v>
-                </pt>
-                <pt idx="1">
-                  <v>0.1158</v>
-                </pt>
-                <pt idx="2">
-                  <v>0.1142</v>
-                </pt>
-                <pt idx="3">
-                  <v>0.1134</v>
-                </pt>
-                <pt idx="4">
-                  <v>0.0926</v>
-                </pt>
-              </numCache>
-            </numRef>
-          </val>
-        </ser>
-        <dLbls>
-          <showLegendKey val="0"/>
-          <showVal val="0"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
-        </dLbls>
-        <gapWidth val="219"/>
-        <overlap val="-27"/>
-        <axId val="202102800"/>
-        <axId val="202103360"/>
-      </barChart>
-      <catAx>
-        <axId val="202102800"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
-        <numFmt formatCode="General" sourceLinked="1"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
-        <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="9525">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-          </a:ln>
-        </spPr>
-        <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="800">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs charset="0" panose="020B0604020202020204" pitchFamily="34" typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:t/>
-            </a:r>
-            <a:endParaRPr lang="lt-LT"/>
-          </a:p>
-        </txPr>
-        <crossAx val="202103360"/>
-        <crosses val="autoZero"/>
-        <auto val="1"/>
-        <lblAlgn val="ctr"/>
-        <lblOffset val="100"/>
-        <noMultiLvlLbl val="0"/>
-      </catAx>
-      <valAx>
-        <axId val="202103360"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <delete val="0"/>
-        <axPos val="l"/>
-        <majorGridlines>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" algn="ctr" cap="flat" cmpd="sng" w="9525">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </spPr>
-        </majorGridlines>
-        <numFmt formatCode="0.00%" sourceLinked="1"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
-        <spPr>
-          <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:noFill/>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </spPr>
-        <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:t/>
-            </a:r>
-            <a:endParaRPr lang="lt-LT"/>
-          </a:p>
-        </txPr>
-        <crossAx val="202102800"/>
+        <crossAx val="220762144"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
@@ -1293,33 +1073,6 @@
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </twoCellAnchor>
-  <twoCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>238125</colOff>
-      <row>98</row>
-      <rowOff>52387</rowOff>
-    </from>
-    <to>
-      <col>12</col>
-      <colOff>542925</colOff>
-      <row>112</row>
-      <rowOff>128587</rowOff>
-    </to>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="4" name="Chart 4"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1595,7 +1348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V114"/>
+  <dimension ref="A1:V80"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="A1" sqref="A1"/>
@@ -1616,7 +1369,7 @@
       </c>
       <c r="K1" s="4" t="inlineStr">
         <is>
-          <t>Nasdaq OMX Baltic Price Performance Highlights</t>
+          <t>Nasdaq OMX Baltic Companies Highlights and Ideas</t>
         </is>
       </c>
     </row>
@@ -1626,56 +1379,56 @@
           <t>RKB1R</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>0.212121212121212</v>
+      <c r="B2" s="7" t="n">
+        <v>0.3000000000000002</v>
       </c>
       <c r="C2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GRD1R</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0.1944444444444444</v>
+          <t>SKN1T</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>0.09090909090909087</v>
       </c>
       <c r="C3" s="1" t="n"/>
       <c r="K3" s="3">
-        <f>B19&amp;" - "&amp;B18</f>
+        <f>"Price Performance "&amp;B19&amp;" - "&amp;B18</f>
         <v/>
       </c>
     </row>
     <row customHeight="1" ht="9.75" r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LJM1R</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0.06666666666666662</v>
+          <t>PKG1T</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>0.08208955223880587</v>
       </c>
       <c r="C4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>OLF1R</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>0.05120481927710855</v>
+          <t>SAB1L</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>0.05756929637526658</v>
       </c>
       <c r="C5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SAB1L</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.0492505353319057</v>
+          <t>UTR1L</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>0.05000000000000004</v>
       </c>
       <c r="C6" s="1" t="n"/>
     </row>
@@ -1692,54 +1445,62 @@
           <t>BLT1T</t>
         </is>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>-0.3125</v>
+      <c r="B8" s="7" t="n">
+        <v>-0.3314763231197771</v>
       </c>
       <c r="C8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INL1L</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>-0.135678391959799</v>
+          <t>SAF1R</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>-0.04761904761904766</v>
       </c>
       <c r="C9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SNG1L</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>-0.0789473684210527</v>
+          <t>TVEAT</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>-0.03508771929824565</v>
       </c>
       <c r="C10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>K2LT</t>
-        </is>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>-0.06060606060606061</v>
+          <t>SMA1R</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>-0.02702702702702703</v>
       </c>
       <c r="C11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RJR1R</t>
-        </is>
-      </c>
-      <c r="B12" s="1" t="n">
-        <v>-0.05670103092783497</v>
+          <t>HAE1T</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>-0.0263736263736264</v>
       </c>
       <c r="C12" s="1" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="8" t="inlineStr">
+        <is>
+          <t>Python input in yellow (except A15:B15)</t>
+        </is>
+      </c>
+      <c r="B15" s="8" t="n"/>
     </row>
     <row customHeight="1" ht="7.5" r="17"/>
     <row customHeight="1" ht="15.75" r="18">
@@ -1750,7 +1511,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2019.07.23</t>
+          <t>2019.07.25</t>
         </is>
       </c>
     </row>
@@ -1762,7 +1523,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2019.07.16</t>
+          <t>2019.07.18</t>
         </is>
       </c>
     </row>
@@ -1774,14 +1535,24 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>P/tBV</t>
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>FCF/Market Cap</t>
         </is>
       </c>
       <c r="B21" s="6">
-        <f>INDEX($B$30:$B$64,MATCH($A$21,$A$30:$A$64,0))</f>
-        <v/>
+        <f>INDEX($B$46:$B$80,MATCH($A$21,$A$46:$A$80,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Sorting</t>
+        </is>
+      </c>
+      <c r="B22" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1790,13 +1561,13 @@
           <t>All types</t>
         </is>
       </c>
-      <c r="U24" t="inlineStr">
+      <c r="U24" s="8" t="inlineStr">
         <is>
           <t>Baltika</t>
         </is>
       </c>
-      <c r="V24" t="n">
-        <v>-0.3752931242532856</v>
+      <c r="V24" s="8" t="n">
+        <v>0.954981654138533</v>
       </c>
     </row>
     <row r="25">
@@ -1805,13 +1576,13 @@
           <t>General</t>
         </is>
       </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>Panevėžio statybos trestas</t>
-        </is>
-      </c>
-      <c r="V25" t="n">
-        <v>0.3405392938018955</v>
+      <c r="U25" s="8" t="inlineStr">
+        <is>
+          <t>Ditton pievadķēžu rūpnīca</t>
+        </is>
+      </c>
+      <c r="V25" s="8" t="n">
+        <v>0.8467367719832509</v>
       </c>
     </row>
     <row r="26">
@@ -1820,13 +1591,13 @@
           <t>Accounting</t>
         </is>
       </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>Kauno energija</t>
-        </is>
-      </c>
-      <c r="V26" t="n">
-        <v>0.4568353691700483</v>
+      <c r="U26" s="8" t="inlineStr">
+        <is>
+          <t>Pieno žvaigždės</t>
+        </is>
+      </c>
+      <c r="V26" s="8" t="n">
+        <v>0.2212177824306152</v>
       </c>
     </row>
     <row r="27">
@@ -1835,253 +1606,79 @@
           <t>Percentage</t>
         </is>
       </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>Linas Agro Group</t>
-        </is>
-      </c>
-      <c r="V27" t="n">
-        <v>0.5806016885843802</v>
+      <c r="U27" s="8" t="inlineStr">
+        <is>
+          <t>Grigeo Grigiškės</t>
+        </is>
+      </c>
+      <c r="V27" s="8" t="n">
+        <v>0.2098183292781833</v>
       </c>
     </row>
     <row r="28">
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>Valmieras stikla šķiedra</t>
-        </is>
-      </c>
-      <c r="V28" t="n">
-        <v>0.6312485621461308</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="inlineStr">
+      <c r="U28" s="8" t="inlineStr">
+        <is>
+          <t>Merko Ehitus</t>
+        </is>
+      </c>
+      <c r="V28" s="8" t="n">
+        <v>0.1917921184686107</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="Q39">
+        <f>"Random metric for the week: "&amp;$A$21</f>
+        <v/>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="40">
+      <c r="Q40" s="5">
+        <f>INDEX($E$46:$F$80,MATCH($A$21,$A$46:$A$80,0),MATCH($B$22,$E$45:$F$45,0))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="O43">
+        <f>U24</f>
+        <v/>
+      </c>
+      <c r="S43">
+        <f>TEXT(V24,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44">
+      <c r="O44">
+        <f>U25</f>
+        <v/>
+      </c>
+      <c r="S44">
+        <f>TEXT(V25,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
         <is>
           <t>Ratio</t>
         </is>
       </c>
-      <c r="B29" s="2" t="inlineStr">
+      <c r="B45" s="2" t="inlineStr">
         <is>
           <t>Format</t>
         </is>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Market Cap., k €</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>EV, k €</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>TOTAL ASSETS</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Book value</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Tangible Book Value</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Minority/Equity</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Intangibles/Equity</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>ROE</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>ROA</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Inventory</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15.75" r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Total Receivables</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Accounting</t>
-        </is>
-      </c>
-      <c r="K40" s="5">
-        <f>"Random metric for the week: "&amp;$A$21</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>D&amp;A/Total Assets</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>D&amp;A/Fixed assets</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>EV/EBITDA</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="I43">
-        <f>U24</f>
-        <v/>
-      </c>
-      <c r="M43">
-        <f>TEXT(V24,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>EV/EBITDA adj.</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="I44">
-        <f>U25</f>
-        <v/>
-      </c>
-      <c r="M44">
-        <f>TEXT(V25,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>P/E</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="I45">
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="O45">
         <f>U26</f>
         <v/>
       </c>
-      <c r="M45">
+      <c r="S45">
         <f>TEXT(V26,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
         <v/>
       </c>
@@ -2089,19 +1686,29 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>P/E adj.</t>
+          <t>Market Cap., k €</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="I46">
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Smallest Companies by Market Cap.</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Largest Companies by Market Cap.</t>
+        </is>
+      </c>
+      <c r="O46">
         <f>U27</f>
         <v/>
       </c>
-      <c r="M46">
+      <c r="S46">
         <f>TEXT(V27,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
         <v/>
       </c>
@@ -2109,19 +1716,29 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>P/tBV</t>
+          <t>EV, k €</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="I47">
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Smallest Companies by Enterprise Value</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Largest Companies by Enterprise Value</t>
+        </is>
+      </c>
+      <c r="O47">
         <f>U28</f>
         <v/>
       </c>
-      <c r="M47">
+      <c r="S47">
         <f>TEXT(V28,IF($B$21=$A$25,"0.00",IF($B$21=$A$26,"#,##0",IF($B$21=$A$27,"0.00%"))))</f>
         <v/>
       </c>
@@ -2129,482 +1746,691 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>NNWC/Market Cap</t>
+          <t>TOTAL ASSETS</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Companies Managing the Least Assets in their Balance Sheets</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Companies Managing most Assets in their Balance Sheets</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Debt/Equity</t>
+          <t>Book value</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
           <t>General</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Smallest Book Values</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Highest Book Values</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Financial debt/Total liabilities</t>
+          <t>Tangible Book Value</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
           <t>General</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Smallest Tangible Book Values</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Highest Tangible Book Values</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Net Debt/EBITDA adj.</t>
+          <t>Minority/Equity</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E51" s="9" t="inlineStr">
+        <is>
+          <t>Least Minority Shareholders Interest</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Highest Minority Shareholders Power in Parent Company</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Current Ratio</t>
+          <t>Intangibles/Equity</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Least Intangible Share in Equity</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Highest Intangible Share in Equity</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Quick Ratio</t>
+          <t>ROE</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Worst Yielding ROE Companies</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Highest Yielding ROE Companies</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Gross profit margin</t>
+          <t>ROA</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
           <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Worst Yielding ROA Companies</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Highest Yielding ROA Companies</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Operating profit margin</t>
+          <t>Inventory</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Percentage</t>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Companies Having Least Inventory</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Companies Having Most Inventory</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Adj. Net profit margin</t>
+          <t>Total Receivables</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Percentage</t>
+          <t>Accounting</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Lowest Supplier Debt (Total Receivables)</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Highest Supplier Debt (Total Receivables)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Adj. EBITDA margin</t>
+          <t>D&amp;A/Total Assets</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Lowest Depreciation &amp; Amortization rate on Total Assets</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Highest Depreciation &amp; Amortization rate on Total Assets</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Cash/Assets</t>
+          <t>D&amp;A/Fixed assets</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
           <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Lowest Depreciation &amp; Amortization rate on Fixed Assets</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Highest Depreciation &amp; Amortization rate on Fixed Assets</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Retained earnings/Assets</t>
+          <t>EV/EBITDA</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Percentage</t>
-        </is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E59">
+        <f>"Most Attractive Companies by "&amp;$A59</f>
+        <v/>
+      </c>
+      <c r="F59">
+        <f>"Most Expensive Companies by "&amp;$A59</f>
+        <v/>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Cash/Retained Earnings</t>
+          <t>EV/EBITDA adj.</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Percentage</t>
-        </is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E60">
+        <f>"Most Attractive Companies by "&amp;$A60</f>
+        <v/>
+      </c>
+      <c r="F60">
+        <f>"Most Expensive Companies by "&amp;$A60</f>
+        <v/>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Cash/Market Cap</t>
+          <t>P/E</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Percentage</t>
-        </is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E61">
+        <f>"Most Attractive Companies by "&amp;$A61</f>
+        <v/>
+      </c>
+      <c r="F61">
+        <f>"Most Expensive Companies by "&amp;$A61</f>
+        <v/>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>FCF/Market Cap</t>
+          <t>P/E adj.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Percentage</t>
-        </is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E62">
+        <f>"Most Attractive Companies by "&amp;$A62</f>
+        <v/>
+      </c>
+      <c r="F62">
+        <f>"Most Expensive Companies by "&amp;$A62</f>
+        <v/>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Dividend yield</t>
+          <t>P/tBV</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Percentage</t>
-        </is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E63">
+        <f>"Most Attractive Companies by "&amp;$A63</f>
+        <v/>
+      </c>
+      <c r="F63">
+        <f>"Most Expensive Companies by "&amp;$A63</f>
+        <v/>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
+          <t>NNWC/Market Cap</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E64">
+        <f>"Worst Deep Value by: "&amp;$A64</f>
+        <v/>
+      </c>
+      <c r="F64">
+        <f>"Best Deep Value by: "&amp;$A64</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Debt/Equity</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Companies with Lowest Financial Leverage (Debt/Equity)</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Companies with Highest Financial Leverage (Debt/Equity)</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Financial debt/Total liabilities</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E66">
+        <f>"Lowest ratio of "&amp;$A66</f>
+        <v/>
+      </c>
+      <c r="F66" s="9">
+        <f>"Highest ratio of "&amp;$A66</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Net Debt/EBITDA adj.</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E67">
+        <f>"Lowest ratio of "&amp;$A67</f>
+        <v/>
+      </c>
+      <c r="F67">
+        <f>"Highest risk of "&amp;$A67</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Current Ratio</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E68">
+        <f>"Worst Credit Liquidity by: "&amp;$A68</f>
+        <v/>
+      </c>
+      <c r="F68">
+        <f>"Best Credit Liquidity by: "&amp;$A68</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Quick Ratio</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="E69">
+        <f>"Worst Credit Liquidity by: "&amp;$A69</f>
+        <v/>
+      </c>
+      <c r="F69">
+        <f>"Best Credit Liquidity by: "&amp;$A69</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Gross profit margin</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E70">
+        <f>"Companies Generating Lowest "&amp;$A70</f>
+        <v/>
+      </c>
+      <c r="F70">
+        <f>"Companies Generating Highest "&amp;$A70</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Operating profit margin</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E71">
+        <f>"Companies Generating Lowest "&amp;$A71</f>
+        <v/>
+      </c>
+      <c r="F71">
+        <f>"Companies Generating Highest "&amp;$A71</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Adj. Net profit margin</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E72">
+        <f>"Companies Generating Lowest "&amp;$A72</f>
+        <v/>
+      </c>
+      <c r="F72">
+        <f>"Companies Generating Highest "&amp;$A72</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Adj. EBITDA margin</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E73">
+        <f>"Companies Generating Lowest "&amp;$A73</f>
+        <v/>
+      </c>
+      <c r="F73">
+        <f>"Companies Generating Highest "&amp;$A73</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Cash/Assets</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Balance Structure: Lowest Share of Cash in Total Assets</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Balance Structure: Highest Share of Cash in Total Assets</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Retained earnings/Assets</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Balance Structure: Least Retained Earnings in Total Assets</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Balance Structure: Highest Accumulated Retained Earnings in Total Assets</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Cash/Retained Earnings</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E76">
+        <f>"Lowest Cash coverage of Retained Earnings ("&amp;$A76&amp;")"</f>
+        <v/>
+      </c>
+      <c r="F76">
+        <f>"Highest Cash coverage of Retained Earnings ("&amp;$A76&amp;")"</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Cash/Market Cap</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E77" s="9" t="inlineStr">
+        <is>
+          <t>Least Attractive Cash in Assets Coverage of Market Cap. (Cash/Market Cap)</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Most Attractive Cash in Assets Coverage of Market Cap. (Cash/Market Cap)</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>FCF/Market Cap</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E78">
+        <f>"Lowest Free Cash Flow Yield ("&amp;$A78&amp;")"</f>
+        <v/>
+      </c>
+      <c r="F78">
+        <f>"Highest Free Cash Flow Yield ("&amp;$A78&amp;")"</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Dividend yield</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="E79" s="9">
+        <f>"Companies With Lowest "&amp;$A79</f>
+        <v/>
+      </c>
+      <c r="F79">
+        <f>"Companies With Highest "&amp;$A79</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>Payout ratio</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>Percentage</t>
         </is>
       </c>
-    </row>
-    <row r="70">
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>Size</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Balance Ratios</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Valuation</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>Liquidity</t>
-        </is>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>Margins</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>Dividend Potential</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>Market Cap., k €</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>Book value</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>EV/EBITDA</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>Debt/Equity</t>
-        </is>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>Gross profit margin</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>Cash/Assets</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>EV, k €</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Tangible Book Value</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>EV/EBITDA adj.</t>
-        </is>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>Financial debt/Total liabilities</t>
-        </is>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>Operating profit margin</t>
-        </is>
-      </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>Retained earnings/Assets</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>TOTAL ASSETS</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Minority/Equity</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>P/E</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>Net Debt/EBITDA adj.</t>
-        </is>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>Adj. Net profit margin</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>Cash/Retained Earnings</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Intangibles/Equity</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>P/E adj.</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>Current Ratio</t>
-        </is>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>Adj. EBITDA margin</t>
-        </is>
-      </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>Cash/Market Cap</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>ROE</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>P/tBV</t>
-        </is>
-      </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>Quick Ratio</t>
-        </is>
-      </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>FCF/Market Cap</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>ROA</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>NNWC/Market Cap</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>Dividend yield</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Inventory</t>
-        </is>
-      </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>Payout ratio</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Total Receivables</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>D&amp;A/Total Assets</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>D&amp;A/Fixed assets</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>Baltika</t>
-        </is>
-      </c>
-      <c r="E110" s="7" t="n">
-        <v>0.1171</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>Grigeo Grigiškės</t>
-        </is>
-      </c>
-      <c r="E111" s="7" t="n">
-        <v>0.1158</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>Telia Lietuva</t>
-        </is>
-      </c>
-      <c r="E112" s="7" t="n">
-        <v>0.1142</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>Linda Nektar</t>
-        </is>
-      </c>
-      <c r="E113" s="7" t="n">
-        <v>0.1134</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>Pieno žvaigždės</t>
-        </is>
-      </c>
-      <c r="E114" s="7" t="n">
-        <v>0.0926</v>
+      <c r="E80" s="9">
+        <f>"Lowest "&amp;$A80</f>
+        <v/>
+      </c>
+      <c r="F80">
+        <f>"Highest "&amp;$A80</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-added another example 'report' -updated documentation with another example
</commit_message>
<xml_diff>
--- a/data/Template.xlsx
+++ b/data/Template.xlsx
@@ -1380,18 +1380,18 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>0.3000000000000002</v>
+        <v>0.3750000000000001</v>
       </c>
       <c r="C2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SKN1T</t>
+          <t>VSS1R</t>
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>0.09090909090909087</v>
+        <v>0.0984848484848484</v>
       </c>
       <c r="C3" s="1" t="n"/>
       <c r="K3" s="3">
@@ -1402,33 +1402,33 @@
     <row customHeight="1" ht="9.75" r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PKG1T</t>
+          <t>SKN1T</t>
         </is>
       </c>
       <c r="B4" s="7" t="n">
-        <v>0.08208955223880587</v>
+        <v>0.09090909090909087</v>
       </c>
       <c r="C4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SAB1L</t>
+          <t>UTR1L</t>
         </is>
       </c>
       <c r="B5" s="7" t="n">
-        <v>0.05756929637526658</v>
+        <v>0.05000000000000004</v>
       </c>
       <c r="C5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>UTR1L</t>
+          <t>PKG1T</t>
         </is>
       </c>
       <c r="B6" s="7" t="n">
-        <v>0.05000000000000004</v>
+        <v>0.04444444444444431</v>
       </c>
       <c r="C6" s="1" t="n"/>
     </row>
@@ -1442,55 +1442,55 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BLT1T</t>
+          <t>TPD1T</t>
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>-0.3314763231197771</v>
+        <v>-0.3870967741935484</v>
       </c>
       <c r="C8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>SAF1R</t>
+          <t>BLT1T</t>
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>-0.04761904761904766</v>
+        <v>-0.2192691029900332</v>
       </c>
       <c r="C9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TVEAT</t>
+          <t>INC1L</t>
         </is>
       </c>
       <c r="B10" s="7" t="n">
-        <v>-0.03508771929824565</v>
+        <v>-0.04878048780487796</v>
       </c>
       <c r="C10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SMA1R</t>
+          <t>OLF1R</t>
         </is>
       </c>
       <c r="B11" s="7" t="n">
-        <v>-0.02702702702702703</v>
+        <v>-0.03380281690140836</v>
       </c>
       <c r="C11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HAE1T</t>
+          <t>NTU1L</t>
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>-0.0263736263736264</v>
+        <v>-0.03267973856209151</v>
       </c>
       <c r="C12" s="1" t="n"/>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2019.07.25</t>
+          <t>2019.07.26</t>
         </is>
       </c>
     </row>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2019.07.18</t>
+          <t>2019.07.19</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1537,7 @@
     <row r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
-          <t>FCF/Market Cap</t>
+          <t>ROE</t>
         </is>
       </c>
       <c r="B21" s="6">
@@ -1563,11 +1563,11 @@
       </c>
       <c r="U24" s="8" t="inlineStr">
         <is>
-          <t>Baltika</t>
+          <t>PATA Saldus</t>
         </is>
       </c>
       <c r="V24" s="8" t="n">
-        <v>0.954981654138533</v>
+        <v>0.4315683497470772</v>
       </c>
     </row>
     <row r="25">
@@ -1578,11 +1578,11 @@
       </c>
       <c r="U25" s="8" t="inlineStr">
         <is>
-          <t>Ditton pievadķēžu rūpnīca</t>
+          <t>Silvano Fashion Group</t>
         </is>
       </c>
       <c r="V25" s="8" t="n">
-        <v>0.8467367719832509</v>
+        <v>0.30216277307756</v>
       </c>
     </row>
     <row r="26">
@@ -1593,11 +1593,11 @@
       </c>
       <c r="U26" s="8" t="inlineStr">
         <is>
-          <t>Pieno žvaigždės</t>
+          <t>Tallinna Vesi</t>
         </is>
       </c>
       <c r="V26" s="8" t="n">
-        <v>0.2212177824306152</v>
+        <v>0.2561233634353408</v>
       </c>
     </row>
     <row r="27">
@@ -1612,17 +1612,17 @@
         </is>
       </c>
       <c r="V27" s="8" t="n">
-        <v>0.2098183292781833</v>
+        <v>0.2324629178656131</v>
       </c>
     </row>
     <row r="28">
       <c r="U28" s="8" t="inlineStr">
         <is>
-          <t>Merko Ehitus</t>
+          <t>MADARA Cosmetics</t>
         </is>
       </c>
       <c r="V28" s="8" t="n">
-        <v>0.1917921184686107</v>
+        <v>0.1933831470361544</v>
       </c>
     </row>
     <row r="39">

</xml_diff>